<commit_message>
Learning Python Scratch - Selenium With python READ, WRITE, FILE UPLOAD, Assertion with Actual Price Expected Price, ETE Testing
</commit_message>
<xml_diff>
--- a/FileUpload_Testing.xlsx
+++ b/FileUpload_Testing.xlsx
@@ -1,96 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parveen\PythonProject_Scratch\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
-  <si>
-    <t>sno</t>
-  </si>
-  <si>
-    <t>fruit_name</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>price</t>
-  </si>
-  <si>
-    <t>season</t>
-  </si>
-  <si>
-    <t>Mango</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Summer</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Winter</t>
-  </si>
-  <si>
-    <t>Papaya</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Kivi</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -109,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -448,138 +444,187 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" ht="15.75" customHeight="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>sno</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>fruit_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>color</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>price</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>season</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mango</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>400</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Summer</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>990</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Winter</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Papaya</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>187</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Spring</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Banana</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Yellow</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>345</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Kivi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>399</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Winter</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" t="n">
         <v>6</v>
       </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>345</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>187</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>69</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6">
-        <v>399</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Orange</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>199</v>
       </c>
-      <c r="E7" t="s">
-        <v>7</v>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Summer</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="A1:E1 A3:E7 A2:C2 E2" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>